<commit_message>
Agregar funcionalidad de registro de asistencia con interfaz web y almacenamiento en Excel
</commit_message>
<xml_diff>
--- a/registro_asistencia.xlsx
+++ b/registro_asistencia.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,7 +610,6 @@
           <t>Entrada</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -628,7 +627,58 @@
           <t>Entrada</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>00:38:39</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>00:38:42</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>00:42:00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Reemplazar archivo de estilos CSS y actualizar registro de asistencia
</commit_message>
<xml_diff>
--- a/registro_asistencia.xlsx
+++ b/registro_asistencia.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -678,7 +678,95 @@
           <t>Entrada</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>00:47:14</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>00:48:23</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>00:49:14</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>00:49:36</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>00:49:42</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Salida</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Actualizar estilos de la interfaz de registro de asistencia y modificar la ruta del archivo CSS
</commit_message>
<xml_diff>
--- a/registro_asistencia.xlsx
+++ b/registro_asistencia.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -712,7 +712,6 @@
           <t>Salida</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -730,7 +729,6 @@
           <t>Salida</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -748,7 +746,6 @@
           <t>Entrada</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -766,7 +763,24 @@
           <t>Salida</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-03-25</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>00:55:11</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>